<commit_message>
updated spreadsheet with insights from evidently
</commit_message>
<xml_diff>
--- a/discovery/problem_stating/generative_ai_cases_from_evidently_selection.xlsx
+++ b/discovery/problem_stating/generative_ai_cases_from_evidently_selection.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t xml:space="preserve">ссылка</t>
   </si>
@@ -40,23 +40,7 @@
     <t xml:space="preserve">как боролись с галюцинациями </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">https://multithreaded.stitchfix.com/blog/2023/03/06/expert-in-the-loop-generative-ai-at-stitch-fix/</t>
-    </r>
+    <t xml:space="preserve"> https://multithreaded.stitchfix.com/blog/2023/03/06/expert-in-the-loop-generative-ai-at-stitch-fix/</t>
   </si>
   <si>
     <t xml:space="preserve">stich fix
@@ -118,6 +102,28 @@
    - ищет в БД похожие кейсы
    - ищет по документации советы и гайды
 И на вход ЛЛМ подавать выход ретривера и описание тикета    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.blog/2023-05-17-inside-github-working-with-the-llms-behind-github-copilot/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GitHub Copilot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- зафайнтюнили гпт3 на куче кода
+- итеративно улучшали промпты</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) на отобранном руками датасете смотрели, дополняет ли модель код правильно или нет
+2) прокси-метрика: как часто юзеры принимают или отклоняют подсказку</t>
+  </si>
+  <si>
+    <t xml:space="preserve">никак, просто пихали в модель кучу кода по аналогии с обычным языком</t>
+  </si>
+  <si>
+    <t xml:space="preserve">модель предлагала для C# конструкции из python:
+1) добавили в промпт название языка программирования
+2) при файнтюне добавляли к файлу его название и расширение</t>
   </si>
 </sst>
 </file>
@@ -132,6 +138,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -153,23 +160,27 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -214,7 +225,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -231,16 +242,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -264,20 +271,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="55.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="32.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="32.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="20.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="21.86"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="24.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -333,8 +340,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="68.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
+    <row r="4" customFormat="false" ht="58.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -343,7 +350,7 @@
       <c r="C4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>18</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -353,11 +360,31 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="77.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6"/>
+    <row r="5" customFormat="false" ht="76.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4"/>
       <c r="B5" s="5"/>
       <c r="C5" s="1" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="104.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -368,7 +395,7 @@
     <mergeCell ref="B4:B5"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://multithreaded.stitchfix.com/blog/2023/03/06/expert-in-the-loop-generative-ai-at-stitch-fix/"/>
+    <hyperlink ref="A2" r:id="rId1" display=" https://multithreaded.stitchfix.com/blog/2023/03/06/expert-in-the-loop-generative-ai-at-stitch-fix/"/>
     <hyperlink ref="A4" r:id="rId2" display="https://www.microsoft.com/en-us/research/blog/large-language-models-for-automatic-cloud-incident-management/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
finalized spreadsheet with insights from evidently. added markdown version
</commit_message>
<xml_diff>
--- a/discovery/problem_stating/generative_ai_cases_from_evidently_selection.xlsx
+++ b/discovery/problem_stating/generative_ai_cases_from_evidently_selection.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="74">
   <si>
     <t xml:space="preserve">ссылка</t>
   </si>
@@ -231,6 +231,82 @@
   </si>
   <si>
     <t xml:space="preserve">не было таких проблем, т.к. по сути использовалась не ЛЛМ, а негенеративная модель </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://medium.com/airbnb-engineering/how-ai-text-generation-models-are-reshaping-customer-support-at-airbnb-a851db0b4fa3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AirBnB
+проект автоматизации customer support</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- подавали на вход запрос юзера и 1 статью из своей базы знаний
+- промптом просили ответить, релевантна ли статья (т.е. только да\нет)
+- в такой постановке зафайнтьюнили MT5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">метрики для классификации, посчитатнные на тестовом датасете
++
+АБ-тест работы на проде</t>
+  </si>
+  <si>
+    <t xml:space="preserve">взяли исторические данные о том как люди-саппортеры общались с клиентами</t>
+  </si>
+  <si>
+    <t xml:space="preserve">не было таких проблем, т.к. свели к классификации</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- отобрали типы вопросов, ответы на которые саппортеры выделяют в тексте обращения
+- зафайнтьюнили модель для Question-Answer общения, но только для этих вопросов
+- для каждого вопроса считали классификационные метрики</t>
+  </si>
+  <si>
+    <t xml:space="preserve">метрики для классификации, посчитатнные на тестовом датасете</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- из всей истории общения с клиентами на основе простой регулярки отобрали  те семплы, где саппортер пытыается перефразировать запрос клиента 
+- кластризовали все парафразы, глазами просмотрели все кластеры и удалили те кластеры, которые содержали слишком общие и неполезные сообщения
+- файнтьюнили T5 модель на парах (запрос клиента) - (парафраз от суппортера)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">не говорят явно
+скорее всего как-то субъективно</t>
+  </si>
+  <si>
+    <t xml:space="preserve">хитро фильтровали историческую выборку</t>
+  </si>
+  <si>
+    <t xml:space="preserve">заморочились с очисткой датасета</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://blog.research.google/2021/10/grammar-correction-as-you-type-on-pixel.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Google
+проект корректировки текста на мобилке</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- наскраппили фраз из интернета
+- прогнали их через большую модель для корректировки
+- на получившемся датасете тренировали с 0 маленькую модель</t>
+  </si>
+  <si>
+    <t xml:space="preserve">не говорят явно
+скорее всего сравнивали выходы маленькой и большой модели</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- использовали публичные данные
+- прогнали их через существующую модель</t>
+  </si>
+  <si>
+    <t xml:space="preserve">проблема с постепенным вводом текста: эвристически определяли, в какой момент разумно делать корректировку и показывать её пользователю</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.grammarly.com/blog/engineering/adversarial-grammatical-error-correction/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">статья про то, как они свели поиск ошибок в тексте к работе GAN’а
+нам не очень релевантно</t>
   </si>
 </sst>
 </file>
@@ -332,7 +408,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -367,6 +443,14 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -386,15 +470,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+      <selection pane="bottomLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.82"/>
@@ -595,12 +679,97 @@
         <v>53</v>
       </c>
     </row>
+    <row r="12" customFormat="false" ht="57.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="9"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="9"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="B12:B14"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display=" https://multithreaded.stitchfix.com/blog/2023/03/06/expert-in-the-loop-generative-ai-at-stitch-fix/"/>

</xml_diff>